<commit_message>
Additional: make JsonUtil generic
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -32,22 +32,22 @@
     <t>Названия университетов</t>
   </si>
   <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t>Московский Выдуманный Университет, Московский Придуманный Институт</t>
+  </si>
+  <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t>Воронежский Литературно-Переводческий Университет</t>
+  </si>
+  <si>
     <t>MATHEMATICS</t>
   </si>
   <si>
     <t>Казанский Университет Вычислений</t>
-  </si>
-  <si>
-    <t>PHYSICS</t>
-  </si>
-  <si>
-    <t>Московский Выдуманный Университет, Московский Придуманный Институт</t>
-  </si>
-  <si>
-    <t>LINGUISTICS</t>
-  </si>
-  <si>
-    <t>Воронежский Литературно-Переводческий Университет</t>
   </si>
   <si>
     <t>MEDICINE</t>
@@ -132,13 +132,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>36.29999923706055</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -149,13 +149,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>36.29999923706055</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>

</xml_diff>